<commit_message>
program no longer prone to malicious input
</commit_message>
<xml_diff>
--- a/grid.xlsx
+++ b/grid.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Uni\Term3\Programming\Dots&amp;Boxes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{94905BFB-B0BA-48E4-A5AB-F8A5C4B131F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D23EE2D-7675-4DE2-841C-6CA963C125E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A18F7325-1298-42DD-9F84-C9381060749F}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8964" xr2:uid="{A18F7325-1298-42DD-9F84-C9381060749F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="4">
   <si>
     <t>o</t>
   </si>
@@ -40,6 +40,9 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>R</t>
   </si>
 </sst>
 </file>
@@ -683,7 +686,7 @@
   <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -763,7 +766,9 @@
         <v>2</v>
       </c>
       <c r="C4" s="14"/>
-      <c r="D4" s="16"/>
+      <c r="D4" s="16" t="s">
+        <v>3</v>
+      </c>
       <c r="E4" s="13"/>
       <c r="F4" s="16"/>
       <c r="G4" s="12" t="s">
@@ -806,7 +811,7 @@
         <v>4</v>
       </c>
       <c r="L5" s="10">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="44.4" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">

</xml_diff>